<commit_message>
correction css base.css et cache prix autom pac retenu
</commit_message>
<xml_diff>
--- a/polls/media/listedepoints.xlsx
+++ b/polls/media/listedepoints.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="25">
   <si>
     <t>Sous-ensemble</t>
   </si>
@@ -34,6 +34,15 @@
     <t>Télé-Commande</t>
   </si>
   <si>
+    <t>Général</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Température extérieure </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Défaut manque d'eau </t>
+  </si>
+  <si>
     <t>Chaudière 1</t>
   </si>
   <si>
@@ -52,25 +61,34 @@
     <t xml:space="preserve">Commande chaudiere </t>
   </si>
   <si>
+    <t>Chaudière 2</t>
+  </si>
+  <si>
     <t>Circuit Régulé 1</t>
   </si>
   <si>
-    <t>Température Ambiant1</t>
-  </si>
-  <si>
-    <t>Commande V3V 1</t>
-  </si>
-  <si>
-    <t>Général</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Température extérieure </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Défaut manque d'eau </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> TOTAUX (14 points)</t>
+    <t>Température  1</t>
+  </si>
+  <si>
+    <t>Température Ambiant 1</t>
+  </si>
+  <si>
+    <t>Défaut pompe  1</t>
+  </si>
+  <si>
+    <t>Commande pompe  1</t>
+  </si>
+  <si>
+    <t>Commande V3V  1</t>
+  </si>
+  <si>
+    <t>Circuit Régulé 2</t>
+  </si>
+  <si>
+    <t>Circuit Régulé 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TOTAUX (32 points)</t>
   </si>
 </sst>
 </file>
@@ -431,7 +449,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -466,11 +484,9 @@
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="B2" s="2"/>
       <c r="C2" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="2">
         <v>0</v>
@@ -488,13 +504,13 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" s="2">
         <v>0</v>
@@ -509,7 +525,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="2">
         <v>0</v>
@@ -527,11 +543,9 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>10</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="B5" s="2"/>
       <c r="C5" s="2">
         <v>0</v>
       </c>
@@ -539,22 +553,22 @@
         <v>0</v>
       </c>
       <c r="E5" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="2">
         <v>0</v>
@@ -563,22 +577,22 @@
         <v>0</v>
       </c>
       <c r="F6" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="2">
         <v>0</v>
@@ -590,16 +604,16 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="C8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="2">
         <v>0</v>
@@ -611,31 +625,31 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C9" s="2">
         <v>0</v>
       </c>
       <c r="D9" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C10" s="2">
         <v>0</v>
@@ -644,7 +658,7 @@
         <v>0</v>
       </c>
       <c r="E10" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10" s="2">
         <v>1</v>
@@ -653,11 +667,9 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>14</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="B11" s="2"/>
       <c r="C11" s="2">
         <v>0</v>
       </c>
@@ -665,7 +677,7 @@
         <v>0</v>
       </c>
       <c r="E11" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11" s="2">
         <v>0</v>
@@ -677,7 +689,7 @@
         <v>15</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C12" s="2">
         <v>1</v>
@@ -698,40 +710,492 @@
         <v>15</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2">
+        <v>1</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0</v>
+      </c>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0</v>
+      </c>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0</v>
+      </c>
+      <c r="E15" s="2">
+        <v>1</v>
+      </c>
+      <c r="F15" s="2">
+        <v>1</v>
+      </c>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0</v>
+      </c>
+      <c r="F16" s="2">
+        <v>1</v>
+      </c>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2">
+        <v>0</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0</v>
+      </c>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="2">
-        <v>0</v>
-      </c>
-      <c r="D13" s="2">
-        <v>1</v>
-      </c>
-      <c r="E13" s="2">
-        <v>0</v>
-      </c>
-      <c r="F13" s="2">
-        <v>0</v>
-      </c>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1" t="s">
+      <c r="C18" s="2">
+        <v>1</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0</v>
+      </c>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="1">
-        <v>4</v>
-      </c>
-      <c r="D14" s="1">
-        <v>4</v>
-      </c>
-      <c r="E14" s="1">
-        <v>3</v>
-      </c>
-      <c r="F14" s="1">
-        <v>3</v>
-      </c>
-      <c r="G14" s="1"/>
+      <c r="C19" s="2">
+        <v>1</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0</v>
+      </c>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0</v>
+      </c>
+      <c r="D20" s="2">
+        <v>1</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0</v>
+      </c>
+      <c r="F20" s="2">
+        <v>0</v>
+      </c>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0</v>
+      </c>
+      <c r="E21" s="2">
+        <v>1</v>
+      </c>
+      <c r="F21" s="2">
+        <v>1</v>
+      </c>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0</v>
+      </c>
+      <c r="E22" s="2">
+        <v>1</v>
+      </c>
+      <c r="F22" s="2">
+        <v>0</v>
+      </c>
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2">
+        <v>0</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0</v>
+      </c>
+      <c r="F23" s="2">
+        <v>0</v>
+      </c>
+      <c r="G23" s="2"/>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="2">
+        <v>1</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0</v>
+      </c>
+      <c r="E24" s="2">
+        <v>0</v>
+      </c>
+      <c r="F24" s="2">
+        <v>0</v>
+      </c>
+      <c r="G24" s="2"/>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" s="2">
+        <v>1</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0</v>
+      </c>
+      <c r="F25" s="2">
+        <v>0</v>
+      </c>
+      <c r="G25" s="2"/>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0</v>
+      </c>
+      <c r="D26" s="2">
+        <v>1</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0</v>
+      </c>
+      <c r="F26" s="2">
+        <v>0</v>
+      </c>
+      <c r="G26" s="2"/>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0</v>
+      </c>
+      <c r="E27" s="2">
+        <v>1</v>
+      </c>
+      <c r="F27" s="2">
+        <v>1</v>
+      </c>
+      <c r="G27" s="2"/>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" s="2">
+        <v>0</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0</v>
+      </c>
+      <c r="E28" s="2">
+        <v>1</v>
+      </c>
+      <c r="F28" s="2">
+        <v>0</v>
+      </c>
+      <c r="G28" s="2"/>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2">
+        <v>0</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0</v>
+      </c>
+      <c r="E29" s="2">
+        <v>0</v>
+      </c>
+      <c r="F29" s="2">
+        <v>0</v>
+      </c>
+      <c r="G29" s="2"/>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" s="2">
+        <v>1</v>
+      </c>
+      <c r="D30" s="2">
+        <v>0</v>
+      </c>
+      <c r="E30" s="2">
+        <v>0</v>
+      </c>
+      <c r="F30" s="2">
+        <v>0</v>
+      </c>
+      <c r="G30" s="2"/>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" s="2">
+        <v>1</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0</v>
+      </c>
+      <c r="E31" s="2">
+        <v>0</v>
+      </c>
+      <c r="F31" s="2">
+        <v>0</v>
+      </c>
+      <c r="G31" s="2"/>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" s="2">
+        <v>0</v>
+      </c>
+      <c r="D32" s="2">
+        <v>1</v>
+      </c>
+      <c r="E32" s="2">
+        <v>0</v>
+      </c>
+      <c r="F32" s="2">
+        <v>0</v>
+      </c>
+      <c r="G32" s="2"/>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" s="2">
+        <v>0</v>
+      </c>
+      <c r="D33" s="2">
+        <v>0</v>
+      </c>
+      <c r="E33" s="2">
+        <v>1</v>
+      </c>
+      <c r="F33" s="2">
+        <v>1</v>
+      </c>
+      <c r="G33" s="2"/>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34" s="2">
+        <v>0</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0</v>
+      </c>
+      <c r="E34" s="2">
+        <v>1</v>
+      </c>
+      <c r="F34" s="2">
+        <v>0</v>
+      </c>
+      <c r="G34" s="2"/>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2">
+        <v>0</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0</v>
+      </c>
+      <c r="E35" s="2">
+        <v>0</v>
+      </c>
+      <c r="F35" s="2">
+        <v>0</v>
+      </c>
+      <c r="G35" s="2"/>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C36" s="1">
+        <v>9</v>
+      </c>
+      <c r="D36" s="1">
+        <v>8</v>
+      </c>
+      <c r="E36" s="1">
+        <v>8</v>
+      </c>
+      <c r="F36" s="1">
+        <v>7</v>
+      </c>
+      <c r="G36" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
1 liste de points par utilisateur, correction pb dowload template
</commit_message>
<xml_diff>
--- a/polls/media/listedepoints.xlsx
+++ b/polls/media/listedepoints.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
   <si>
     <t>Sous-ensemble</t>
   </si>
@@ -61,7 +61,7 @@
     <t xml:space="preserve">Commande chaudiere </t>
   </si>
   <si>
-    <t>Chaudière 2</t>
+    <t>Divers 1</t>
   </si>
   <si>
     <t>Circuit Régulé 1</t>
@@ -85,10 +85,10 @@
     <t>Circuit Régulé 2</t>
   </si>
   <si>
-    <t>Circuit Régulé 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> TOTAUX (32 points)</t>
+    <t>zzzzeTOTAL</t>
+  </si>
+  <si>
+    <t>TOTAUX (23 points)</t>
   </si>
 </sst>
 </file>
@@ -449,7 +449,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -484,9 +484,11 @@
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="C2" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" s="2">
         <v>0</v>
@@ -504,13 +506,13 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" s="2">
         <v>0</v>
@@ -522,16 +524,16 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C4" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" s="2">
         <v>0</v>
@@ -545,12 +547,14 @@
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="C5" s="2">
         <v>0</v>
       </c>
       <c r="D5" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="2">
         <v>0</v>
@@ -565,13 +569,13 @@
         <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C6" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" s="2">
         <v>0</v>
@@ -586,19 +590,19 @@
         <v>9</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C7" s="2">
         <v>0</v>
       </c>
       <c r="D7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" s="2"/>
     </row>
@@ -607,49 +611,49 @@
         <v>9</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C8" s="2">
         <v>0</v>
       </c>
       <c r="D8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" s="2">
         <v>0</v>
       </c>
       <c r="F8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" s="2">
         <v>0</v>
       </c>
       <c r="D9" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" s="2">
         <v>0</v>
@@ -658,7 +662,7 @@
         <v>0</v>
       </c>
       <c r="E10" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" s="2">
         <v>1</v>
@@ -667,11 +671,13 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="2"/>
+        <v>16</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="C11" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" s="2">
         <v>0</v>
@@ -686,10 +692,10 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C12" s="2">
         <v>1</v>
@@ -707,10 +713,10 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C13" s="2">
         <v>0</v>
@@ -728,31 +734,31 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C14" s="2">
         <v>0</v>
       </c>
       <c r="D14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C15" s="2">
         <v>0</v>
@@ -764,19 +770,19 @@
         <v>1</v>
       </c>
       <c r="F15" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" s="2">
         <v>0</v>
@@ -785,17 +791,19 @@
         <v>0</v>
       </c>
       <c r="F16" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="2"/>
+        <v>22</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="C17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" s="2">
         <v>0</v>
@@ -810,16 +818,16 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" s="2">
         <v>0</v>
@@ -831,40 +839,40 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C19" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19" s="2">
         <v>0</v>
       </c>
       <c r="E19" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C20" s="2">
         <v>0</v>
       </c>
       <c r="D20" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E20" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20" s="2">
         <v>0</v>
@@ -872,330 +880,25 @@
       <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21" s="2">
-        <v>0</v>
-      </c>
-      <c r="D21" s="2">
-        <v>0</v>
-      </c>
-      <c r="E21" s="2">
-        <v>1</v>
-      </c>
-      <c r="F21" s="2">
-        <v>1</v>
-      </c>
-      <c r="G21" s="2"/>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="2">
-        <v>0</v>
-      </c>
-      <c r="D22" s="2">
-        <v>0</v>
-      </c>
-      <c r="E22" s="2">
-        <v>1</v>
-      </c>
-      <c r="F22" s="2">
-        <v>0</v>
-      </c>
-      <c r="G22" s="2"/>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2">
-        <v>0</v>
-      </c>
-      <c r="D23" s="2">
-        <v>0</v>
-      </c>
-      <c r="E23" s="2">
-        <v>0</v>
-      </c>
-      <c r="F23" s="2">
-        <v>0</v>
-      </c>
-      <c r="G23" s="2"/>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C24" s="2">
-        <v>1</v>
-      </c>
-      <c r="D24" s="2">
-        <v>0</v>
-      </c>
-      <c r="E24" s="2">
-        <v>0</v>
-      </c>
-      <c r="F24" s="2">
-        <v>0</v>
-      </c>
-      <c r="G24" s="2"/>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C25" s="2">
-        <v>1</v>
-      </c>
-      <c r="D25" s="2">
-        <v>0</v>
-      </c>
-      <c r="E25" s="2">
-        <v>0</v>
-      </c>
-      <c r="F25" s="2">
-        <v>0</v>
-      </c>
-      <c r="G25" s="2"/>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C26" s="2">
-        <v>0</v>
-      </c>
-      <c r="D26" s="2">
-        <v>1</v>
-      </c>
-      <c r="E26" s="2">
-        <v>0</v>
-      </c>
-      <c r="F26" s="2">
-        <v>0</v>
-      </c>
-      <c r="G26" s="2"/>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C27" s="2">
-        <v>0</v>
-      </c>
-      <c r="D27" s="2">
-        <v>0</v>
-      </c>
-      <c r="E27" s="2">
-        <v>1</v>
-      </c>
-      <c r="F27" s="2">
-        <v>1</v>
-      </c>
-      <c r="G27" s="2"/>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C28" s="2">
-        <v>0</v>
-      </c>
-      <c r="D28" s="2">
-        <v>0</v>
-      </c>
-      <c r="E28" s="2">
-        <v>1</v>
-      </c>
-      <c r="F28" s="2">
-        <v>0</v>
-      </c>
-      <c r="G28" s="2"/>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" s="2" t="s">
+      <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2">
-        <v>0</v>
-      </c>
-      <c r="D29" s="2">
-        <v>0</v>
-      </c>
-      <c r="E29" s="2">
-        <v>0</v>
-      </c>
-      <c r="F29" s="2">
-        <v>0</v>
-      </c>
-      <c r="G29" s="2"/>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="A30" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C30" s="2">
-        <v>1</v>
-      </c>
-      <c r="D30" s="2">
-        <v>0</v>
-      </c>
-      <c r="E30" s="2">
-        <v>0</v>
-      </c>
-      <c r="F30" s="2">
-        <v>0</v>
-      </c>
-      <c r="G30" s="2"/>
-    </row>
-    <row r="31" spans="1:7">
-      <c r="A31" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C31" s="2">
-        <v>1</v>
-      </c>
-      <c r="D31" s="2">
-        <v>0</v>
-      </c>
-      <c r="E31" s="2">
-        <v>0</v>
-      </c>
-      <c r="F31" s="2">
-        <v>0</v>
-      </c>
-      <c r="G31" s="2"/>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="A32" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C32" s="2">
-        <v>0</v>
-      </c>
-      <c r="D32" s="2">
-        <v>1</v>
-      </c>
-      <c r="E32" s="2">
-        <v>0</v>
-      </c>
-      <c r="F32" s="2">
-        <v>0</v>
-      </c>
-      <c r="G32" s="2"/>
-    </row>
-    <row r="33" spans="1:7">
-      <c r="A33" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C33" s="2">
-        <v>0</v>
-      </c>
-      <c r="D33" s="2">
-        <v>0</v>
-      </c>
-      <c r="E33" s="2">
-        <v>1</v>
-      </c>
-      <c r="F33" s="2">
-        <v>1</v>
-      </c>
-      <c r="G33" s="2"/>
-    </row>
-    <row r="34" spans="1:7">
-      <c r="A34" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C34" s="2">
-        <v>0</v>
-      </c>
-      <c r="D34" s="2">
-        <v>0</v>
-      </c>
-      <c r="E34" s="2">
-        <v>1</v>
-      </c>
-      <c r="F34" s="2">
-        <v>0</v>
-      </c>
-      <c r="G34" s="2"/>
-    </row>
-    <row r="35" spans="1:7">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2">
-        <v>0</v>
-      </c>
-      <c r="D35" s="2">
-        <v>0</v>
-      </c>
-      <c r="E35" s="2">
-        <v>0</v>
-      </c>
-      <c r="F35" s="2">
-        <v>0</v>
-      </c>
-      <c r="G35" s="2"/>
-    </row>
-    <row r="36" spans="1:7">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C36" s="1">
-        <v>9</v>
-      </c>
-      <c r="D36" s="1">
-        <v>8</v>
-      </c>
-      <c r="E36" s="1">
-        <v>8</v>
-      </c>
-      <c r="F36" s="1">
-        <v>7</v>
-      </c>
-      <c r="G36" s="1"/>
+      <c r="C21" s="1">
+        <v>6</v>
+      </c>
+      <c r="D21" s="1">
+        <v>6</v>
+      </c>
+      <c r="E21" s="1">
+        <v>6</v>
+      </c>
+      <c r="F21" s="1">
+        <v>5</v>
+      </c>
+      <c r="G21" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
ajout des compteurs Mbus, Modbus Imp dans la liste de pts
</commit_message>
<xml_diff>
--- a/polls/media/listedepoints.xlsx
+++ b/polls/media/listedepoints.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="31">
   <si>
     <t>Sous-ensemble</t>
   </si>
@@ -34,6 +34,12 @@
     <t>Télé-Commande</t>
   </si>
   <si>
+    <t>Mbus</t>
+  </si>
+  <si>
+    <t>Modbus</t>
+  </si>
+  <si>
     <t>Général</t>
   </si>
   <si>
@@ -46,7 +52,7 @@
     <t>Chaudière 1</t>
   </si>
   <si>
-    <t>Temp 1</t>
+    <t>Température 1</t>
   </si>
   <si>
     <t>Synthèse défaut 1</t>
@@ -61,10 +67,46 @@
     <t xml:space="preserve">Commande chaudiere </t>
   </si>
   <si>
+    <t>Chaudière 2</t>
+  </si>
+  <si>
+    <t>Chaudière 3</t>
+  </si>
+  <si>
+    <t>Chaudière 4</t>
+  </si>
+  <si>
+    <t>Circuit Régulé 1</t>
+  </si>
+  <si>
+    <t>Température  1</t>
+  </si>
+  <si>
+    <t>Température Ambiant 1</t>
+  </si>
+  <si>
+    <t>Défaut pompe  1</t>
+  </si>
+  <si>
+    <t>Commande pompe  1</t>
+  </si>
+  <si>
+    <t>Commande V3V  1</t>
+  </si>
+  <si>
+    <t>Circuit Régulé 2</t>
+  </si>
+  <si>
+    <t>Compteurs</t>
+  </si>
+  <si>
+    <t>Compteur Mbus 1</t>
+  </si>
+  <si>
     <t>zzzzeTOTAL</t>
   </si>
   <si>
-    <t>TOTAUX (8 points)</t>
+    <t>TOTAUX (38 points)</t>
   </si>
 </sst>
 </file>
@@ -425,17 +467,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="60.7109375" customWidth="1"/>
-    <col min="3" max="6" width="20.7109375" customWidth="1"/>
+    <col min="3" max="8" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -454,14 +496,20 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
@@ -475,154 +523,904 @@
       <c r="F2" s="2">
         <v>0</v>
       </c>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="G2" s="2">
+        <v>0</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0</v>
+      </c>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0</v>
+      </c>
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0</v>
+      </c>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0</v>
+      </c>
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0</v>
+      </c>
+      <c r="I10" s="2"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0</v>
+      </c>
+      <c r="I11" s="2"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1</v>
+      </c>
+      <c r="G12" s="2">
+        <v>0</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0</v>
+      </c>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0</v>
+      </c>
+      <c r="F13" s="2">
+        <v>1</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0</v>
+      </c>
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0</v>
+      </c>
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0</v>
+      </c>
+      <c r="D15" s="2">
+        <v>1</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0</v>
+      </c>
+      <c r="G15" s="2">
+        <v>0</v>
+      </c>
+      <c r="H15" s="2">
+        <v>0</v>
+      </c>
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0</v>
+      </c>
+      <c r="D16" s="2">
+        <v>1</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0</v>
+      </c>
+      <c r="G16" s="2">
+        <v>0</v>
+      </c>
+      <c r="H16" s="2">
+        <v>0</v>
+      </c>
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0</v>
+      </c>
+      <c r="E17" s="2">
+        <v>1</v>
+      </c>
+      <c r="F17" s="2">
+        <v>1</v>
+      </c>
+      <c r="G17" s="2">
+        <v>0</v>
+      </c>
+      <c r="H17" s="2">
+        <v>0</v>
+      </c>
+      <c r="I17" s="2"/>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0</v>
+      </c>
+      <c r="F18" s="2">
+        <v>1</v>
+      </c>
+      <c r="G18" s="2">
+        <v>0</v>
+      </c>
+      <c r="H18" s="2">
+        <v>0</v>
+      </c>
+      <c r="I18" s="2"/>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="2">
+        <v>1</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0</v>
+      </c>
+      <c r="G19" s="2">
+        <v>0</v>
+      </c>
+      <c r="H19" s="2">
+        <v>0</v>
+      </c>
+      <c r="I19" s="2"/>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0</v>
+      </c>
+      <c r="D20" s="2">
+        <v>1</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0</v>
+      </c>
+      <c r="F20" s="2">
+        <v>0</v>
+      </c>
+      <c r="G20" s="2">
+        <v>0</v>
+      </c>
+      <c r="H20" s="2">
+        <v>0</v>
+      </c>
+      <c r="I20" s="2"/>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0</v>
+      </c>
+      <c r="D21" s="2">
+        <v>1</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0</v>
+      </c>
+      <c r="F21" s="2">
+        <v>0</v>
+      </c>
+      <c r="G21" s="2">
+        <v>0</v>
+      </c>
+      <c r="H21" s="2">
+        <v>0</v>
+      </c>
+      <c r="I21" s="2"/>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0</v>
+      </c>
+      <c r="E22" s="2">
+        <v>1</v>
+      </c>
+      <c r="F22" s="2">
+        <v>1</v>
+      </c>
+      <c r="G22" s="2">
+        <v>0</v>
+      </c>
+      <c r="H22" s="2">
+        <v>0</v>
+      </c>
+      <c r="I22" s="2"/>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0</v>
+      </c>
+      <c r="F23" s="2">
+        <v>1</v>
+      </c>
+      <c r="G23" s="2">
+        <v>0</v>
+      </c>
+      <c r="H23" s="2">
+        <v>0</v>
+      </c>
+      <c r="I23" s="2"/>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="2">
+        <v>1</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0</v>
+      </c>
+      <c r="E24" s="2">
+        <v>0</v>
+      </c>
+      <c r="F24" s="2">
+        <v>0</v>
+      </c>
+      <c r="G24" s="2">
+        <v>0</v>
+      </c>
+      <c r="H24" s="2">
+        <v>0</v>
+      </c>
+      <c r="I24" s="2"/>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="2">
+        <v>1</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0</v>
+      </c>
+      <c r="F25" s="2">
+        <v>0</v>
+      </c>
+      <c r="G25" s="2">
+        <v>0</v>
+      </c>
+      <c r="H25" s="2">
+        <v>0</v>
+      </c>
+      <c r="I25" s="2"/>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0</v>
+      </c>
+      <c r="D26" s="2">
+        <v>1</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0</v>
+      </c>
+      <c r="F26" s="2">
+        <v>0</v>
+      </c>
+      <c r="G26" s="2">
+        <v>0</v>
+      </c>
+      <c r="H26" s="2">
+        <v>0</v>
+      </c>
+      <c r="I26" s="2"/>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0</v>
+      </c>
+      <c r="E27" s="2">
+        <v>1</v>
+      </c>
+      <c r="F27" s="2">
+        <v>1</v>
+      </c>
+      <c r="G27" s="2">
+        <v>0</v>
+      </c>
+      <c r="H27" s="2">
+        <v>0</v>
+      </c>
+      <c r="I27" s="2"/>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="2">
+        <v>0</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0</v>
+      </c>
+      <c r="E28" s="2">
+        <v>1</v>
+      </c>
+      <c r="F28" s="2">
+        <v>0</v>
+      </c>
+      <c r="G28" s="2">
+        <v>0</v>
+      </c>
+      <c r="H28" s="2">
+        <v>0</v>
+      </c>
+      <c r="I28" s="2"/>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" s="2">
+        <v>1</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0</v>
+      </c>
+      <c r="E29" s="2">
+        <v>0</v>
+      </c>
+      <c r="F29" s="2">
+        <v>0</v>
+      </c>
+      <c r="G29" s="2">
+        <v>0</v>
+      </c>
+      <c r="H29" s="2">
+        <v>0</v>
+      </c>
+      <c r="I29" s="2"/>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30" s="2">
+        <v>1</v>
+      </c>
+      <c r="D30" s="2">
+        <v>0</v>
+      </c>
+      <c r="E30" s="2">
+        <v>0</v>
+      </c>
+      <c r="F30" s="2">
+        <v>0</v>
+      </c>
+      <c r="G30" s="2">
+        <v>0</v>
+      </c>
+      <c r="H30" s="2">
+        <v>0</v>
+      </c>
+      <c r="I30" s="2"/>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" s="2">
+        <v>0</v>
+      </c>
+      <c r="D31" s="2">
+        <v>1</v>
+      </c>
+      <c r="E31" s="2">
+        <v>0</v>
+      </c>
+      <c r="F31" s="2">
+        <v>0</v>
+      </c>
+      <c r="G31" s="2">
+        <v>0</v>
+      </c>
+      <c r="H31" s="2">
+        <v>0</v>
+      </c>
+      <c r="I31" s="2"/>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" s="2">
+        <v>0</v>
+      </c>
+      <c r="D32" s="2">
+        <v>0</v>
+      </c>
+      <c r="E32" s="2">
+        <v>1</v>
+      </c>
+      <c r="F32" s="2">
+        <v>1</v>
+      </c>
+      <c r="G32" s="2">
+        <v>0</v>
+      </c>
+      <c r="H32" s="2">
+        <v>0</v>
+      </c>
+      <c r="I32" s="2"/>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" s="2">
+        <v>0</v>
+      </c>
+      <c r="D33" s="2">
+        <v>0</v>
+      </c>
+      <c r="E33" s="2">
+        <v>1</v>
+      </c>
+      <c r="F33" s="2">
+        <v>0</v>
+      </c>
+      <c r="G33" s="2">
+        <v>0</v>
+      </c>
+      <c r="H33" s="2">
+        <v>0</v>
+      </c>
+      <c r="I33" s="2"/>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C34" s="2">
+        <v>0</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0</v>
+      </c>
+      <c r="E34" s="2">
+        <v>0</v>
+      </c>
+      <c r="F34" s="2">
+        <v>0</v>
+      </c>
+      <c r="G34" s="2">
+        <v>4</v>
+      </c>
+      <c r="H34" s="2">
+        <v>0</v>
+      </c>
+      <c r="I34" s="2"/>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35" s="1">
+        <v>9</v>
+      </c>
+      <c r="D35" s="1">
+        <v>11</v>
+      </c>
+      <c r="E35" s="1">
         <v>8</v>
       </c>
-      <c r="C3" s="2">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2">
-        <v>1</v>
-      </c>
-      <c r="E3" s="2">
-        <v>0</v>
-      </c>
-      <c r="F3" s="2">
-        <v>0</v>
-      </c>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="F35" s="1">
         <v>10</v>
       </c>
-      <c r="C4" s="2">
-        <v>1</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0</v>
-      </c>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="2">
-        <v>0</v>
-      </c>
-      <c r="D5" s="2">
-        <v>1</v>
-      </c>
-      <c r="E5" s="2">
-        <v>0</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0</v>
-      </c>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="2">
-        <v>0</v>
-      </c>
-      <c r="D6" s="2">
-        <v>1</v>
-      </c>
-      <c r="E6" s="2">
-        <v>0</v>
-      </c>
-      <c r="F6" s="2">
-        <v>0</v>
-      </c>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="2">
-        <v>0</v>
-      </c>
-      <c r="D7" s="2">
-        <v>0</v>
-      </c>
-      <c r="E7" s="2">
-        <v>1</v>
-      </c>
-      <c r="F7" s="2">
-        <v>1</v>
-      </c>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="2">
-        <v>0</v>
-      </c>
-      <c r="D8" s="2">
-        <v>0</v>
-      </c>
-      <c r="E8" s="2">
-        <v>0</v>
-      </c>
-      <c r="F8" s="2">
-        <v>1</v>
-      </c>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="1">
-        <v>2</v>
-      </c>
-      <c r="D9" s="1">
-        <v>3</v>
-      </c>
-      <c r="E9" s="1">
-        <v>1</v>
-      </c>
-      <c r="F9" s="1">
-        <v>2</v>
-      </c>
-      <c r="G9" s="1"/>
+      <c r="G35" s="1">
+        <v>4</v>
+      </c>
+      <c r="H35" s="1">
+        <v>0</v>
+      </c>
+      <c r="I35" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
prise en compte Mbus liste pour config WIT
</commit_message>
<xml_diff>
--- a/polls/media/listedepoints.xlsx
+++ b/polls/media/listedepoints.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="33">
   <si>
     <t>Sous-ensemble</t>
   </si>
@@ -103,10 +103,16 @@
     <t>Compteur Mbus 1</t>
   </si>
   <si>
+    <t>Compteur Modbus 1</t>
+  </si>
+  <si>
+    <t>Compteur Impul 1</t>
+  </si>
+  <si>
     <t>zzzzeTOTAL</t>
   </si>
   <si>
-    <t>TOTAUX (38 points)</t>
+    <t>TOTAUX (53 points)</t>
   </si>
 </sst>
 </file>
@@ -467,7 +473,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1396,31 +1402,85 @@
       <c r="I34" s="2"/>
     </row>
     <row r="35" spans="1:9">
-      <c r="A35" s="1" t="s">
+      <c r="A35" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="C35" s="2">
+        <v>0</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0</v>
+      </c>
+      <c r="E35" s="2">
+        <v>0</v>
+      </c>
+      <c r="F35" s="2">
+        <v>0</v>
+      </c>
+      <c r="G35" s="2">
+        <v>0</v>
+      </c>
+      <c r="H35" s="2">
+        <v>10</v>
+      </c>
+      <c r="I35" s="2"/>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C36" s="2">
+        <v>0</v>
+      </c>
+      <c r="D36" s="2">
+        <v>1</v>
+      </c>
+      <c r="E36" s="2">
+        <v>0</v>
+      </c>
+      <c r="F36" s="2">
+        <v>0</v>
+      </c>
+      <c r="G36" s="2">
+        <v>0</v>
+      </c>
+      <c r="H36" s="2">
+        <v>0</v>
+      </c>
+      <c r="I36" s="2"/>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C37" s="1">
         <v>9</v>
       </c>
-      <c r="D35" s="1">
-        <v>11</v>
-      </c>
-      <c r="E35" s="1">
+      <c r="D37" s="1">
+        <v>12</v>
+      </c>
+      <c r="E37" s="1">
         <v>8</v>
       </c>
-      <c r="F35" s="1">
+      <c r="F37" s="1">
         <v>10</v>
       </c>
-      <c r="G35" s="1">
+      <c r="G37" s="1">
         <v>4</v>
       </c>
-      <c r="H35" s="1">
-        <v>0</v>
-      </c>
-      <c r="I35" s="1"/>
+      <c r="H37" s="1">
+        <v>10</v>
+      </c>
+      <c r="I37" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>